<commit_message>
finished handling patient data with excel 'NO TEST APPLIED' i guess!. separted the commone used excel methods in its own class
</commit_message>
<xml_diff>
--- a/exel files/EmployeeData.xlsx
+++ b/exel files/EmployeeData.xlsx
@@ -1,27 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\codez\uni projects\hospital system my work\exel files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9D4E77-7B0B-43BD-B746-CF33C622068F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PreviousExperience" sheetId="1" r:id="rId1"/>
-    <sheet name="NumberOfEmployee" sheetId="2" r:id="rId4"/>
-    <sheet name="Manger" sheetId="3" r:id="rId5"/>
-    <sheet name="HR" sheetId="4" r:id="rId6"/>
-    <sheet name="Accountant" sheetId="5" r:id="rId7"/>
-    <sheet name="Receptionist" sheetId="6" r:id="rId8"/>
-    <sheet name="Doctor" sheetId="7" r:id="rId9"/>
-    <sheet name="Nurse" sheetId="8" r:id="rId10"/>
-    <sheet name="Radiologist" sheetId="9" r:id="rId11"/>
-    <sheet name="Pharmacist" sheetId="10" r:id="rId12"/>
+    <sheet name="NumberOfEmployee" sheetId="2" r:id="rId2"/>
+    <sheet name="Manger" sheetId="3" r:id="rId3"/>
+    <sheet name="HR" sheetId="4" r:id="rId4"/>
+    <sheet name="Accountant" sheetId="5" r:id="rId5"/>
+    <sheet name="Receptionist" sheetId="6" r:id="rId6"/>
+    <sheet name="Doctor" sheetId="7" r:id="rId7"/>
+    <sheet name="Nurse" sheetId="8" r:id="rId8"/>
+    <sheet name="Radiologist" sheetId="9" r:id="rId9"/>
+    <sheet name="Pharmacist" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>ID</t>
   </si>
@@ -176,21 +195,21 @@
     <t>A+</t>
   </si>
   <si>
+    <t>08:00:00</t>
+  </si>
+  <si>
+    <t>01-Jan-23</t>
+  </si>
+  <si>
+    <t>CIB</t>
+  </si>
+  <si>
+    <t>1234-2345-3456-4567</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>01-Jan-23</t>
-  </si>
-  <si>
-    <t>CIB</t>
-  </si>
-  <si>
-    <t>1234-2345-3456-4567</t>
-  </si>
-  <si>
-    <t>28-Jun-24 2:49:08 AM</t>
-  </si>
-  <si>
     <t>Abdullah Elrouby</t>
   </si>
   <si>
@@ -200,25 +219,13 @@
     <t>Egypt. Behira. Wadi-Elnatrun</t>
   </si>
   <si>
-    <t>28-Jun-24 2:23:51 AM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abdullah Elrouby logged in at 24-Jun-24 10:31:26 PM
-Abdullah Elrouby logged out at 24-Jun-24 10:30:16 PM
-Abdullah Elrouby today work hours -00:01:10
-another worning sent.
-Abdullah Elrouby has 1 warnings now
-HR : Abdullah Elrouby
-Date : 24-Jun-24 10:33:18 PM</t>
+    <t>29-Jun-24 6:25:34 AM</t>
   </si>
   <si>
     <t>Mahmoud Bakr</t>
   </si>
   <si>
     <t>Egypt. Alexandria. Borj Al-arab</t>
-  </si>
-  <si>
-    <t>27-Jun-24 10:36:24 PM</t>
   </si>
   <si>
     <t>Heba-Allah Mohamed</t>
@@ -254,7 +261,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="4">
     <font>
@@ -297,110 +304,23 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
-    <xf numFmtId="0" fontId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" applyAlignment="1">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" applyFont="1" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" applyFont="1" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" applyFont="1" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" applyFont="1" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" applyFont="1" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" applyFont="1" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" applyFont="1" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" applyFont="1" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" applyFont="1" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -408,17 +328,320 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName=""/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
@@ -508,1326 +731,1332 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName=""/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="20" t="s">
+      <c r="C1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="O1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="P1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" s="20" t="s">
+      <c r="Q1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="R1" s="20" t="s">
+      <c r="R1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="S1" s="20" t="s">
+      <c r="S1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="T1" s="20" t="s">
+      <c r="T1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="U1" s="20" t="s">
+      <c r="U1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="V1" s="20" t="s">
+      <c r="V1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="W1" s="20" t="s">
+      <c r="W1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="X1" s="20" t="s">
+      <c r="X1" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="1">
+        <v>20</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" s="1">
+        <v>11000</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" s="19">
-        <v>20</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="K2" s="19">
-        <v>11000</v>
-      </c>
-      <c r="L2" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="M2" s="19" t="s">
+      <c r="M2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N2" s="19">
+      <c r="N2" s="1">
         <v>1</v>
       </c>
-      <c r="O2" s="19" t="s">
+      <c r="O2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="P2" s="19" t="s">
+      <c r="P2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="Q2" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="R2" s="19" t="s">
+      <c r="Q2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="19">
-        <v>0</v>
-      </c>
-      <c r="T2" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="U2" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="V2" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="W2" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="X2" s="19">
+      <c r="S2" s="1">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="X2" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName=""/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="15">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="19">
+      <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="1">
         <v>1</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="1">
         <f>SUM(A2:G2)</f>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName=""/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="V1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W1" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="1">
         <v>20</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="1">
         <v>20000</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2" s="1">
         <v>1</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="P2" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q2" s="5" t="s">
+      <c r="P2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="5">
-        <v>0</v>
-      </c>
-      <c r="S2" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="T2" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="V2" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="W2" s="5">
+      <c r="R2" s="1">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="W2" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName=""/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="W1" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="1">
         <v>20</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J2" s="21">
-        <v>12000</v>
-      </c>
-      <c r="K2" s="7" t="s">
+      <c r="J2" s="1">
+        <v>10000</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="M2" s="7">
+      <c r="M2" s="1">
         <v>1</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="P2" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q2" s="7" t="s">
+      <c r="P2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="7">
-        <v>0</v>
-      </c>
-      <c r="S2" s="31" t="s">
+      <c r="R2" s="1">
+        <v>0</v>
+      </c>
+      <c r="S2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="T2" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="U2" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="V2" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="W2" s="7">
+      <c r="T2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="W2" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName=""/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="Q1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="V1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="W1" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="1">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="9">
-        <v>20</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J2" s="9">
-        <v>90000</v>
-      </c>
-      <c r="K2" s="9" t="s">
+      <c r="J2" s="1">
+        <v>9000</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="M2" s="9">
+      <c r="M2" s="1">
         <v>1</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="O2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="P2" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q2" s="9" t="s">
+      <c r="P2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="9">
-        <v>0</v>
-      </c>
-      <c r="S2" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="T2" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="U2" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="V2" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="W2" s="9">
+      <c r="R2" s="1">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="W2" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName=""/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="O1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="P1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="Q1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="R1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="S1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="T1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="U1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="V1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="W1" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="1">
         <v>23</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="I2" s="11" t="s">
+      <c r="H2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J2" s="11">
-        <v>60000</v>
-      </c>
-      <c r="K2" s="11" t="s">
+      <c r="J2" s="1">
+        <v>6000</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="M2" s="11">
+      <c r="M2" s="1">
         <v>1</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="N2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="O2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="P2" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q2" s="11" t="s">
+      <c r="P2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="11">
-        <v>0</v>
-      </c>
-      <c r="S2" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="U2" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="V2" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="W2" s="11">
+      <c r="R2" s="1">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="W2" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName=""/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="Q1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="R1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S1" s="14" t="s">
+      <c r="S1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="T1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="U1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="V1" s="14" t="s">
+      <c r="V1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W1" s="14" t="s">
+      <c r="W1" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="1">
         <v>20</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="I2" s="13" t="s">
+      <c r="H2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J2" s="13">
+      <c r="J2" s="1">
         <v>15000</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="M2" s="13">
+      <c r="M2" s="1">
         <v>1</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="N2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="O2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="P2" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q2" s="13" t="s">
+      <c r="P2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="13">
-        <v>0</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="T2" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="U2" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="V2" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="W2" s="13">
+      <c r="R2" s="1">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="W2" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName=""/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="O1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="P1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="Q1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="16" t="s">
+      <c r="R1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="S1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="T1" s="16" t="s">
+      <c r="T1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="U1" s="16" t="s">
+      <c r="U1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="V1" s="16" t="s">
+      <c r="V1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W1" s="16" t="s">
+      <c r="W1" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="15" t="s">
+      <c r="B2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="1">
         <v>20</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="I2" s="15" t="s">
+      <c r="H2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J2" s="15">
+      <c r="J2" s="1">
         <v>12500</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="M2" s="15">
+      <c r="M2" s="1">
         <v>1</v>
       </c>
-      <c r="N2" s="15" t="s">
+      <c r="N2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="O2" s="15" t="s">
+      <c r="O2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="P2" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q2" s="15" t="s">
+      <c r="P2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="15">
-        <v>0</v>
-      </c>
-      <c r="S2" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="T2" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="U2" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="V2" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="W2" s="15">
+      <c r="R2" s="1">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="W2" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName=""/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="N1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="O1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="P1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="18" t="s">
+      <c r="Q1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="18" t="s">
+      <c r="R1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S1" s="18" t="s">
+      <c r="S1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="T1" s="18" t="s">
+      <c r="T1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="U1" s="18" t="s">
+      <c r="U1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="V1" s="18" t="s">
+      <c r="V1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W1" s="18" t="s">
+      <c r="W1" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="17" t="s">
+      <c r="B2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="1">
         <v>20</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="I2" s="17" t="s">
+      <c r="H2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J2" s="17">
+      <c r="J2" s="1">
         <v>14000</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="M2" s="17">
+      <c r="M2" s="1">
         <v>1</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="O2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="P2" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q2" s="17" t="s">
+      <c r="P2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="17">
-        <v>0</v>
-      </c>
-      <c r="S2" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="T2" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="U2" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="V2" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="W2" s="17">
+      <c r="R2" s="1">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="W2" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>